<commit_message>
added convert json file to excell file
</commit_message>
<xml_diff>
--- a/resources/files/Sample_output.xlsx
+++ b/resources/files/Sample_output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sadashivareddys\Downloads\BDD_UI-main\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8596047A-6234-4FFD-A338-8155D3864255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67554174-5B6B-448A-90E4-296C31718F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,42 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>engagementKey</t>
+    <t>organization</t>
   </si>
   <si>
-    <t>characteristics</t>
-  </si>
-  <si>
-    <t>wardKey</t>
-  </si>
-  <si>
-    <t>actionKey</t>
-  </si>
-  <si>
-    <t>actionTakenOn</t>
-  </si>
-  <si>
-    <t>participantKey</t>
-  </si>
-  <si>
-    <t>&lt;engagementKey&gt;</t>
-  </si>
-  <si>
-    <t>{"state":"AZ"}</t>
-  </si>
-  <si>
-    <t>&lt;wardKey&gt;</t>
-  </si>
-  <si>
-    <t>&lt;actionKey&gt;</t>
-  </si>
-  <si>
-    <t>2021-11-23T08:14:22.981-07:00</t>
-  </si>
-  <si>
-    <t>&lt;participantKey&gt;</t>
+    <t>{"dunsControlStatus":{"detailedOperatingStatus":{},"subjectHandlingDetails":[],"isSelfRequestedDUNS":null,"isDelisted":false,"isMailUndeliverable":false,"firstReportDate":null,"operatingSubStatus":{"description":"Active","dnbCode":9074,"startDate":null},"isMarketable":true,"isTelephoneDisconnected":null,"operatingStatus":{"description":"Active","dnbCode":9074,"startDate":null},"selfRequestDate":null,"recordClass":{}},"websiteAddress":[],"industrialPlantsCount":null,"stockExchanges":[],"globalUltimate":{},"registeredAddress":{},"multilingualPrimaryAddress":[],"isAgent":null,"multilingualTradestyleNames":[],"defaultCurrency":"INR","employerDesignation":{},"incorporatedDate":"2021-05-25","domesticUltimate":{},"isSmallBusiness":null,"certifiedEmail":null,"multilingualRegisteredAddress":[],"financials":[{"informationScopeDnBCode":null,"informationScopeDescription":null,"financialStatementToDate":null,"yearlyRevenue":[{"currency":"INR","value":198168709},{"currency":"USD","value":2360982}],"reliabilityDnBCode":9094,"unitCode":"SingleUnits","financialStatementDuration":null,"reliabilityDescription":"Modelled"}],"registeredDetails":{"legalForm":{"registrationStatus":{},"description":"Private Limited Liability Company","dnbCode":12903,"localLegalForms":[]}},"businessTrustIndex":{},"multiLingualSearchNames":[],"standardizedStockExchanges":[],"banks":[],"telephone":[],"registrationNumbers":[{"registrationLocation":null,"registrationNumber":"AAGCE4803L","typeDnBCode":12897,"registrationNumberClass":{"description":"Fiscal / Tax Registration Number","dnbCode":2929},"isPreferredRegistrationNumber":null,"typeDescription":"Tax Identification Number (IN)"},{"registrationLocation":null,"registrationNumber":"U72900KA2021FTC147805","typeDnBCode":1362,"registrationNumberClass":{"description":"National Business Registration Number","dnbCode":2888},"isPreferredRegistrationNumber":null,"typeDescription":"Company Incorporation Number (IN)"}],"numberOfEmployees":[{"employeeFiguresDate":"2023-07-31","informationScopeDnBCode":9067,"informationScopeDescription":"Consolidated","trend":[],"reliabilityDnBCode":9092,"employeeCategories":[],"value":26,"reliabilityDescription":"Actual"},{"employeeFiguresDate":"2023-07-31","informationScopeDnBCode":9066,"informationScopeDescription":"Individual","reliabilityDnBCode":9092,"employeeCategories":[],"value":26,"reliabilityDescription":"Actual"}],"tradeStyleNames":[],"registeredName":"EXOSTAR INDIA PRIVATE LIMITED","duns":"854404636","primaryAddress":{"addressCountry":{"name":"India","isoAlpha2Code":"IN"},"postalCodePosition":{"description":"Post Code presented after Town/City name","dnbCode":1011},"geographicalPrecision":{"description":"Postal Code Centroid","dnbCode":30258},"minorTownName":null,"streetNumber":null,"continentalRegion":{"name":"Asia Pacific"},"postalCode":"560010","isRegisteredAddress":true,"latitude":12.99877,"language":{"description":"English","dnbCode":39},"addressCounty":{},"postalRoute":null,"streetName":null,"postOfficeBox":{},"isManufacturingLocation":null,"standardAddressCodes":[],"streetAddress":{"line2":"Dr. Rajkumar Road, Rajajinagar","line1":"Regus, Tejas Arcade #527/b, 3rd &amp; 4th Floor 1st Main Road"},"statisticalArea":{},"addressLocality":{"name":"Bengaluru"},"addressRegion":{"isoSubDivisionCode":"IN-KA","name":"Karnataka","administrativeDivisionCode":null,"isoSubDivisionName":"Karnataka","abbreviatedName":"KA"},"longitude":77.57331},"startDate":"2021-05-25","primaryIndustryCode":{"usSicV4":"7379","usSicV4Description":"Computer related services"},"isExporter":null,"preferredLanguage":{"description":"English","dnbCode":39},"isFortune1000Listed":null,"controlOwnershipDate":"2021-05-25","industryCodes":[{"code":"541512","typeDnBCode":37788,"description":"Computer Systems Design Services","typeDescription":"North American Industry Classification System 2022","priority":1},{"code":"73790000","typeDnBCode":3599,"description":"Computer related services, nec","typeDescription":"D&amp;B Standard Industry Code","priority":1},{"code":"6203","typeDnBCode":29104,"description":"Computer facilities management activities","typeDescription":"NACE Revision 2","priority":1},{"code":"7379","typeDnBCode":399,"description":"Computer related services","typeDescription":"US Standard Industry Code 1987 - 4 digit","priority":1},{"code":"42","typeDnBCode":35912,"description":"Computer System Design Services","typeDescription":"D&amp;B Hoovers Industry Classification","priority":1},{"code":"I","typeDnBCode":24657,"description":"Services","typeDescription":"D&amp;B Standard Major Industry Code","priority":1},{"code":"6202","typeDnBCode":42726,"description":"Computer consultancy and computer facilities management activities","typeDescription":"ISIC Revision 4","priority":1}],"imperialCalendarStartYear":null,"countryISOAlpha2Code":"IN","multilingualPrimaryName":[],"fiscalYearEnd":null,"organizationSizeCategory":{},"corporateLinkage":{},"isImporter":null,"unspscCodes":[{"code":"81110000","description":"Computer services","priority":1}],"isStandalone":true,"isForbesLargestPrivateCompaniesListed":null,"tsrReportDate":null,"controlOwnershipType":{},"email":[{"address":"sudeep.dharan@exostar.com"}],"summary":[],"legalEntityIdentifier":null,"securitiesReportID":null,"businessEntityType":{"description":"Corporation","dnbCode":451},"primaryName":"EXOSTAR INDIA PRIVATE LIMITED","legalForm":{"registrationLocation":{},"description":"Private Limited Company","dnbCode":31148,"startDate":"2021-05-25"},"charterType":{},"mailingAddress":{},"activities":[],"isNonClassifiedEstablishment":null,"multilingualRegisteredNames":[],"subjectComments":[],"investigationDate":null}</t>
   </si>
 </sst>
 </file>
@@ -427,58 +397,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="255.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>